<commit_message>
bug fixed and started with outputting all the questions
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julia\Desktop\hs17-bewertete-uebung-JuHa11\docs\exercise\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="28800" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="16215" yWindow="28800" windowWidth="25365" windowHeight="15825" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$32</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -162,11 +167,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,12 +260,20 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -589,16 +602,16 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9">
@@ -660,10 +673,7 @@
         <f>SUM(G4:G5)</f>
         <v>20</v>
       </c>
-      <c r="H6" s="4">
-        <f>MIN(C6,G6)</f>
-        <v>20</v>
-      </c>
+      <c r="H6" s="4"/>
     </row>
     <row r="8" spans="2:9">
       <c r="D8">
@@ -731,10 +741,7 @@
         <f>SUM(G8:G12)</f>
         <v>22</v>
       </c>
-      <c r="H13" s="4">
-        <f>MIN(C13,G13)</f>
-        <v>15</v>
-      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="2"/>
@@ -828,10 +835,7 @@
         <f>SUM(G15:G21)</f>
         <v>20</v>
       </c>
-      <c r="H22" s="4">
-        <f>MIN(C22,G22)</f>
-        <v>15</v>
-      </c>
+      <c r="H22" s="4"/>
     </row>
     <row r="24" spans="2:9">
       <c r="D24">
@@ -899,10 +903,7 @@
         <f>SUM(G24:G28)</f>
         <v>25</v>
       </c>
-      <c r="H29" s="4">
-        <f>MIN(C29,G29)</f>
-        <v>5</v>
-      </c>
+      <c r="H29" s="4"/>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="3" t="s">
@@ -913,11 +914,11 @@
       </c>
       <c r="H32">
         <f>SUM(H4:H29)</f>
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <f>MIN(C32,H32)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:9">
@@ -932,7 +933,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="6">
         <f>1 + TOTAL_POINTS/10</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
at least one answer has to be chosen in the quiz
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16215" yWindow="28800" windowWidth="25365" windowHeight="15825" tabRatio="500"/>
+    <workbookView xWindow="16220" yWindow="28800" windowWidth="25370" windowHeight="15830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$32</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -598,20 +598,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9">

</xml_diff>